<commit_message>
Context: I am trying to create the student progress report for Denise/faculty. This requires aggregation of student and note data, and required some extra fields to be added to the student schema.
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>onyen</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>FA 2019</t>
+  </si>
+  <si>
+    <t>technicalWritingApproved</t>
+  </si>
+  <si>
+    <t>programProductRequirement</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,20 +525,22 @@
     <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" customWidth="1"/>
+    <col min="24" max="24" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.140625" customWidth="1"/>
+    <col min="28" max="28" width="25" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,40 +608,46 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -704,7 +718,7 @@
         <v>43726</v>
       </c>
       <c r="X2" s="2">
-        <v>43726.833333333336</v>
+        <v>43726</v>
       </c>
       <c r="Y2" s="2">
         <v>43726.833333333336</v>
@@ -713,24 +727,30 @@
         <v>43726.833333333336</v>
       </c>
       <c r="AA2" s="2">
+        <v>43726</v>
+      </c>
+      <c r="AB2" s="2">
         <v>43726.833333333336</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>43497.833333333336</v>
       </c>
       <c r="AC2" s="2">
         <v>43726.833333333336</v>
       </c>
       <c r="AD2" s="2">
-        <v>43726.833333333336</v>
+        <v>43497.833333333336</v>
       </c>
       <c r="AE2" s="2">
         <v>43726.833333333336</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Context: Trying to automatically calculate whether students are guaranteed or not if they go over 10 semesters. So added semesters on leave field to students, and on the student edit page added javascript to auto calculate fundingStatus based on semesterStarted and semestersOnLeave. Also fixed small bug that was making student lastnames and firstnames uppercase in the upload function.
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>onyen</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>programProductRequirement</t>
+  </si>
+  <si>
+    <t>semestersOnLeave</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,25 +525,26 @@
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" customWidth="1"/>
-    <col min="24" max="24" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.140625" customWidth="1"/>
-    <col min="28" max="28" width="25" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" customWidth="1"/>
+    <col min="25" max="25" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.140625" customWidth="1"/>
+    <col min="29" max="29" width="25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,55 +603,58 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -705,41 +712,41 @@
       <c r="S2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
+        <v>99</v>
+      </c>
+      <c r="U2" s="2">
         <v>43726</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>43497.833333333336</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>43726.833333333336</v>
-      </c>
-      <c r="W2" s="2">
-        <v>43726</v>
       </c>
       <c r="X2" s="2">
         <v>43726</v>
       </c>
       <c r="Y2" s="2">
-        <v>43726.833333333336</v>
+        <v>43726</v>
       </c>
       <c r="Z2" s="2">
         <v>43726.833333333336</v>
       </c>
       <c r="AA2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AB2" s="2">
         <v>43726</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>43726.833333333336</v>
       </c>
       <c r="AC2" s="2">
         <v>43726.833333333336</v>
       </c>
       <c r="AD2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AE2" s="2">
         <v>43497.833333333336</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>43726.833333333336</v>
       </c>
       <c r="AF2" s="2">
         <v>43726.833333333336</v>
@@ -747,10 +754,13 @@
       <c r="AG2" s="2">
         <v>43726.833333333336</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added otherAdvisor option and applied necessary changes elsewhere
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun\Desktop\CS-Grad-Tracking\data\InOrderUploadTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonjunjin/CS-Grad-Tracking/data/InOrderUploadTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FACB03-81D5-487B-B962-40A1EA4B1074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA26CBC-9648-E246-8C0F-363E9B5C211E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>onyen</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>semestersOnLeave</t>
+  </si>
+  <si>
+    <t>otherAdvisor</t>
   </si>
 </sst>
 </file>
@@ -500,52 +503,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.26171875" customWidth="1"/>
-    <col min="21" max="21" width="20.26171875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.15625" customWidth="1"/>
-    <col min="25" max="25" width="34.68359375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.15625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.15625" customWidth="1"/>
+    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" customWidth="1"/>
+    <col min="21" max="21" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1640625" customWidth="1"/>
+    <col min="25" max="25" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.1640625" customWidth="1"/>
     <col min="29" max="29" width="25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.68359375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,8 +658,11 @@
       <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AK1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
created two advisor fields for both research and academic
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonjunjin/CS-Grad-Tracking/data/InOrderUploadTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA26CBC-9648-E246-8C0F-363E9B5C211E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654706FF-BD75-8741-BDD2-426E34B58FD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>onyen</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>otherAdvisor</t>
+  </si>
+  <si>
+    <t>researchAdvisor</t>
+  </si>
+  <si>
+    <t>otherResearchAdvisor</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,9 +553,11 @@
     <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.6640625" customWidth="1"/>
+    <col min="38" max="38" width="18.83203125" customWidth="1"/>
+    <col min="39" max="39" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,8 +669,14 @@
       <c r="AK1" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -769,6 +783,9 @@
         <v>48</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor fixes to the stateresidency and USresidency changes
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonjunjin/CS-Grad-Tracking/data/InOrderUploadTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654706FF-BD75-8741-BDD2-426E34B58FD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6A3B3-A677-3E47-A7C9-93F73DB04B55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>onyen</t>
   </si>
@@ -60,9 +60,6 @@
     <t>ethnicity</t>
   </si>
   <si>
-    <t>residency</t>
-  </si>
-  <si>
     <t>enteringStatus</t>
   </si>
   <si>
@@ -190,6 +187,12 @@
   </si>
   <si>
     <t>otherResearchAdvisor</t>
+  </si>
+  <si>
+    <t>stateResidency</t>
+  </si>
+  <si>
+    <t>USResidency</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -527,37 +530,38 @@
     <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.33203125" customWidth="1"/>
-    <col min="21" max="21" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.1640625" customWidth="1"/>
-    <col min="25" max="25" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.1640625" customWidth="1"/>
-    <col min="29" max="29" width="25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.6640625" customWidth="1"/>
-    <col min="38" max="38" width="18.83203125" customWidth="1"/>
-    <col min="39" max="39" width="18.5" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.1640625" customWidth="1"/>
+    <col min="26" max="26" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.1640625" customWidth="1"/>
+    <col min="30" max="30" width="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" customWidth="1"/>
+    <col min="39" max="39" width="18.83203125" customWidth="1"/>
+    <col min="40" max="40" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,186 +596,189 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>949949949</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1">
+        <v>20</v>
+      </c>
+      <c r="S2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="1">
-        <v>20</v>
-      </c>
-      <c r="R2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>99</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>43726</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>43497.833333333336</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>43726.833333333336</v>
-      </c>
-      <c r="X2" s="2">
-        <v>43726</v>
       </c>
       <c r="Y2" s="2">
         <v>43726</v>
       </c>
       <c r="Z2" s="2">
-        <v>43726.833333333336</v>
+        <v>43726</v>
       </c>
       <c r="AA2" s="2">
         <v>43726.833333333336</v>
       </c>
       <c r="AB2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AC2" s="2">
         <v>43726</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>43726.833333333336</v>
       </c>
       <c r="AD2" s="2">
         <v>43726.833333333336</v>
       </c>
       <c r="AE2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="AF2" s="2">
         <v>43497.833333333336</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>43726.833333333336</v>
       </c>
       <c r="AG2" s="2">
         <v>43726.833333333336</v>
@@ -779,14 +786,17 @@
       <c r="AH2" s="2">
         <v>43726.833333333336</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>48</v>
+      <c r="AI2" s="2">
+        <v>43726.833333333336</v>
       </c>
       <c r="AJ2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL2" t="s">
-        <v>47</v>
+      <c r="AK2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited columns in excel to match csv
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonjunjin/CS-Grad-Tracking/data/InOrderUploadTests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elaine\CS-Grad-Tracking\data\InOrderUploadTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6A3B3-A677-3E47-A7C9-93F73DB04B55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A675C8F0-A3E1-4D67-A23C-A93F95B6B182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2256" yWindow="3012" windowWidth="20220" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>onyen</t>
   </si>
@@ -51,30 +51,15 @@
     <t>status</t>
   </si>
   <si>
-    <t>alternativeName</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
     <t>ethnicity</t>
   </si>
   <si>
-    <t>enteringStatus</t>
-  </si>
-  <si>
-    <t>researchArea</t>
-  </si>
-  <si>
-    <t>leaveExtension</t>
-  </si>
-  <si>
     <t>intendedDegree</t>
   </si>
   <si>
-    <t>hoursCompleted</t>
-  </si>
-  <si>
     <t>citizenship</t>
   </si>
   <si>
@@ -84,42 +69,15 @@
     <t>backgroundApproved</t>
   </si>
   <si>
-    <t>mastersAwarded</t>
-  </si>
-  <si>
     <t>prpPassed</t>
   </si>
   <si>
-    <t>backgroundPrepWorksheetApproved</t>
-  </si>
-  <si>
-    <t>programOfStudyApproved</t>
-  </si>
-  <si>
-    <t>researchPlanningMeeting</t>
-  </si>
-  <si>
     <t>committeeCompApproved</t>
   </si>
   <si>
-    <t>phdProposalApproved</t>
-  </si>
-  <si>
-    <t>phdAwarded</t>
-  </si>
-  <si>
     <t>oralExamPassed</t>
   </si>
   <si>
-    <t>dissertationDefencePassed</t>
-  </si>
-  <si>
-    <t>dissertationSubmitted</t>
-  </si>
-  <si>
-    <t>semesterStarted</t>
-  </si>
-  <si>
     <t>advisor</t>
   </si>
   <si>
@@ -150,15 +108,6 @@
     <t>YES</t>
   </si>
   <si>
-    <t>help</t>
-  </si>
-  <si>
-    <t>Systems</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>MASTERS</t>
   </si>
   <si>
@@ -168,31 +117,22 @@
     <t>test, test</t>
   </si>
   <si>
-    <t>FA 2019</t>
-  </si>
-  <si>
-    <t>technicalWritingApproved</t>
-  </si>
-  <si>
-    <t>programProductRequirement</t>
-  </si>
-  <si>
-    <t>semestersOnLeave</t>
-  </si>
-  <si>
-    <t>otherAdvisor</t>
-  </si>
-  <si>
     <t>researchAdvisor</t>
   </si>
   <si>
-    <t>otherResearchAdvisor</t>
-  </si>
-  <si>
     <t>stateResidency</t>
   </si>
   <si>
     <t>USResidency</t>
+  </si>
+  <si>
+    <t>msProgramOfStudyApproved</t>
+  </si>
+  <si>
+    <t>phdProgramOfStudyApproved</t>
+  </si>
+  <si>
+    <t>phdProposaApproved</t>
   </si>
 </sst>
 </file>
@@ -512,56 +452,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" customWidth="1"/>
-    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.1640625" customWidth="1"/>
-    <col min="26" max="26" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.1640625" customWidth="1"/>
-    <col min="30" max="30" width="25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.6640625" customWidth="1"/>
-    <col min="39" max="39" width="18.83203125" customWidth="1"/>
-    <col min="40" max="40" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.77734375" customWidth="1"/>
+    <col min="25" max="25" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,13 +518,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -614,189 +539,100 @@
         <v>14</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G2" s="1">
         <v>949949949</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="1">
-        <v>20</v>
-      </c>
-      <c r="S2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="1">
-        <v>99</v>
+        <v>28</v>
+      </c>
+      <c r="P2" s="2">
+        <v>43726</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="R2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="S2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="T2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="U2" s="2">
+        <v>43726.833333333336</v>
       </c>
       <c r="V2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="W2" s="2">
-        <v>43497.833333333336</v>
-      </c>
-      <c r="X2" s="2">
         <v>43726.833333333336</v>
       </c>
-      <c r="Y2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>43497.833333333336</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>46</v>
+      <c r="W2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typo in excel test sheet
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/2studentUpload.xlsx
+++ b/data/InOrderUploadTests/2studentUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonjunjin/CS-Grad-Tracking/data/InOrderUploadTests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elaine\CS-Grad-Tracking\data\InOrderUploadTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6A3B3-A677-3E47-A7C9-93F73DB04B55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3679FE-128A-495C-8DE2-16C0281D7C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>onyen</t>
   </si>
@@ -51,30 +51,15 @@
     <t>status</t>
   </si>
   <si>
-    <t>alternativeName</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
     <t>ethnicity</t>
   </si>
   <si>
-    <t>enteringStatus</t>
-  </si>
-  <si>
-    <t>researchArea</t>
-  </si>
-  <si>
-    <t>leaveExtension</t>
-  </si>
-  <si>
     <t>intendedDegree</t>
   </si>
   <si>
-    <t>hoursCompleted</t>
-  </si>
-  <si>
     <t>citizenship</t>
   </si>
   <si>
@@ -84,115 +69,70 @@
     <t>backgroundApproved</t>
   </si>
   <si>
-    <t>mastersAwarded</t>
-  </si>
-  <si>
     <t>prpPassed</t>
   </si>
   <si>
-    <t>backgroundPrepWorksheetApproved</t>
-  </si>
-  <si>
-    <t>programOfStudyApproved</t>
-  </si>
-  <si>
-    <t>researchPlanningMeeting</t>
-  </si>
-  <si>
     <t>committeeCompApproved</t>
   </si>
   <si>
+    <t>oralExamPassed</t>
+  </si>
+  <si>
+    <t>advisor</t>
+  </si>
+  <si>
+    <t>fakeonyen</t>
+  </si>
+  <si>
+    <t>fakecsid</t>
+  </si>
+  <si>
+    <t>fakeEmail@fake.com</t>
+  </si>
+  <si>
+    <t>fake</t>
+  </si>
+  <si>
+    <t>she, her</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>MASTERS</t>
+  </si>
+  <si>
+    <t>GUARANTEED</t>
+  </si>
+  <si>
+    <t>test, test</t>
+  </si>
+  <si>
+    <t>researchAdvisor</t>
+  </si>
+  <si>
+    <t>stateResidency</t>
+  </si>
+  <si>
+    <t>USResidency</t>
+  </si>
+  <si>
+    <t>msProgramOfStudyApproved</t>
+  </si>
+  <si>
+    <t>phdProgramOfStudyApproved</t>
+  </si>
+  <si>
     <t>phdProposalApproved</t>
-  </si>
-  <si>
-    <t>phdAwarded</t>
-  </si>
-  <si>
-    <t>oralExamPassed</t>
-  </si>
-  <si>
-    <t>dissertationDefencePassed</t>
-  </si>
-  <si>
-    <t>dissertationSubmitted</t>
-  </si>
-  <si>
-    <t>semesterStarted</t>
-  </si>
-  <si>
-    <t>advisor</t>
-  </si>
-  <si>
-    <t>fakeonyen</t>
-  </si>
-  <si>
-    <t>fakecsid</t>
-  </si>
-  <si>
-    <t>fakeEmail@fake.com</t>
-  </si>
-  <si>
-    <t>fake</t>
-  </si>
-  <si>
-    <t>she, her</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>help</t>
-  </si>
-  <si>
-    <t>Systems</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>MASTERS</t>
-  </si>
-  <si>
-    <t>GUARANTEED</t>
-  </si>
-  <si>
-    <t>test, test</t>
-  </si>
-  <si>
-    <t>FA 2019</t>
-  </si>
-  <si>
-    <t>technicalWritingApproved</t>
-  </si>
-  <si>
-    <t>programProductRequirement</t>
-  </si>
-  <si>
-    <t>semestersOnLeave</t>
-  </si>
-  <si>
-    <t>otherAdvisor</t>
-  </si>
-  <si>
-    <t>researchAdvisor</t>
-  </si>
-  <si>
-    <t>otherResearchAdvisor</t>
-  </si>
-  <si>
-    <t>stateResidency</t>
-  </si>
-  <si>
-    <t>USResidency</t>
   </si>
 </sst>
 </file>
@@ -512,56 +452,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" customWidth="1"/>
-    <col min="22" max="22" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.1640625" customWidth="1"/>
-    <col min="26" max="26" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.1640625" customWidth="1"/>
-    <col min="30" max="30" width="25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.6640625" customWidth="1"/>
-    <col min="39" max="39" width="18.83203125" customWidth="1"/>
-    <col min="40" max="40" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.77734375" customWidth="1"/>
+    <col min="25" max="25" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,13 +518,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -614,189 +539,100 @@
         <v>14</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G2" s="1">
         <v>949949949</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="1">
-        <v>20</v>
-      </c>
-      <c r="S2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="1">
-        <v>99</v>
+        <v>28</v>
+      </c>
+      <c r="P2" s="2">
+        <v>43726</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="R2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="S2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="T2" s="2">
+        <v>43726.833333333336</v>
+      </c>
+      <c r="U2" s="2">
+        <v>43726.833333333336</v>
       </c>
       <c r="V2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="W2" s="2">
-        <v>43497.833333333336</v>
-      </c>
-      <c r="X2" s="2">
         <v>43726.833333333336</v>
       </c>
-      <c r="Y2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>43726</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>43497.833333333336</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>43726.833333333336</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>46</v>
+      <c r="W2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>